<commit_message>
patients update 20201015 2226
</commit_message>
<xml_diff>
--- a/work/09_tochigi.xlsx
+++ b/work/09_tochigi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\06-01②総務G（広報チーム）\HP更新用\発生状況一覧\20201014\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\06-01②総務G（広報チーム）\HP更新用\発生状況一覧\20201015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">発生状況!$A$2:$H$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">発生状況!$A$1:$H$458</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">発生状況!$A$1:$H$459</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">発生状況!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="620">
   <si>
     <t>栃木県内　新型コロナウイルス感染症　発生状況</t>
   </si>
@@ -5231,6 +5231,14 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5956,11 +5964,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H458"/>
+  <dimension ref="A1:H459"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I448" sqref="I448"/>
+      <pane ySplit="2" topLeftCell="A444" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F457" sqref="F457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5971,7 +5979,8 @@
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
     <col min="6" max="7" width="11.625" style="3" customWidth="1"/>
     <col min="8" max="8" width="48.75" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="5.75" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -16653,8 +16662,8 @@
       <c r="F412" s="20">
         <v>44097</v>
       </c>
-      <c r="G412" s="18" t="s">
-        <v>583</v>
+      <c r="G412" s="20">
+        <v>44118</v>
       </c>
       <c r="H412" s="24" t="s">
         <v>583</v>
@@ -16757,8 +16766,8 @@
       <c r="F416" s="20">
         <v>44098</v>
       </c>
-      <c r="G416" s="18" t="s">
-        <v>583</v>
+      <c r="G416" s="20">
+        <v>44119</v>
       </c>
       <c r="H416" s="24" t="s">
         <v>549</v>
@@ -17355,8 +17364,8 @@
       <c r="F439" s="36">
         <v>44107</v>
       </c>
-      <c r="G439" s="27" t="s">
-        <v>587</v>
+      <c r="G439" s="36">
+        <v>44116</v>
       </c>
       <c r="H439" s="28" t="s">
         <v>589</v>
@@ -17485,8 +17494,8 @@
       <c r="F444" s="20">
         <v>44110</v>
       </c>
-      <c r="G444" s="18" t="s">
-        <v>583</v>
+      <c r="G444" s="20">
+        <v>44116</v>
       </c>
       <c r="H444" s="24" t="s">
         <v>602</v>
@@ -17512,7 +17521,7 @@
         <v>44110</v>
       </c>
       <c r="G445" s="20">
-        <v>44116</v>
+        <v>44115</v>
       </c>
       <c r="H445" s="24" t="s">
         <v>604</v>
@@ -17537,8 +17546,8 @@
       <c r="F446" s="20">
         <v>44110</v>
       </c>
-      <c r="G446" s="20">
-        <v>44115</v>
+      <c r="G446" s="20" t="s">
+        <v>619</v>
       </c>
       <c r="H446" s="24" t="s">
         <v>603</v>
@@ -17564,7 +17573,7 @@
         <v>44111</v>
       </c>
       <c r="G447" s="18" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="H447" s="24" t="s">
         <v>583</v>
@@ -17615,237 +17624,263 @@
       <c r="F449" s="20">
         <v>44113</v>
       </c>
-      <c r="G449" s="18" t="s">
-        <v>583</v>
+      <c r="G449" s="20">
+        <v>44119</v>
       </c>
       <c r="H449" s="24" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="450" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A450" s="55">
+      <c r="A450" s="18">
         <v>445</v>
       </c>
-      <c r="B450" s="55">
+      <c r="B450" s="18">
         <v>446</v>
       </c>
-      <c r="C450" s="56" t="s">
+      <c r="C450" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="D450" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E450" s="55" t="s">
+      <c r="D450" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E450" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="F450" s="58">
+      <c r="F450" s="20">
         <v>44117</v>
       </c>
-      <c r="G450" s="55" t="s">
+      <c r="G450" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H450" s="59" t="s">
+      <c r="H450" s="24" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="451" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A451" s="55">
+      <c r="A451" s="18">
         <v>446</v>
       </c>
-      <c r="B451" s="55">
+      <c r="B451" s="18">
         <v>447</v>
       </c>
-      <c r="C451" s="56" t="s">
+      <c r="C451" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D451" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E451" s="55" t="s">
+      <c r="D451" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E451" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F451" s="58">
+      <c r="F451" s="20">
         <v>44117</v>
       </c>
-      <c r="G451" s="55" t="s">
+      <c r="G451" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H451" s="59" t="s">
+      <c r="H451" s="24" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="452" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A452" s="55">
+      <c r="A452" s="18">
         <v>447</v>
       </c>
-      <c r="B452" s="55">
+      <c r="B452" s="18">
         <v>448</v>
       </c>
-      <c r="C452" s="56" t="s">
+      <c r="C452" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D452" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E452" s="55" t="s">
+      <c r="D452" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E452" s="18" t="s">
         <v>609</v>
       </c>
-      <c r="F452" s="58">
+      <c r="F452" s="20">
         <v>44118</v>
       </c>
-      <c r="G452" s="55" t="s">
+      <c r="G452" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H452" s="59" t="s">
+      <c r="H452" s="24" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="453" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A453" s="55">
+      <c r="A453" s="18">
         <v>448</v>
       </c>
-      <c r="B453" s="55">
+      <c r="B453" s="18">
         <v>449</v>
       </c>
-      <c r="C453" s="56" t="s">
+      <c r="C453" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D453" s="57" t="s">
+      <c r="D453" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E453" s="55" t="s">
+      <c r="E453" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F453" s="58">
+      <c r="F453" s="20">
         <v>44118</v>
       </c>
-      <c r="G453" s="55" t="s">
+      <c r="G453" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H453" s="59" t="s">
+      <c r="H453" s="24" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="454" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A454" s="55">
+      <c r="A454" s="18">
         <v>449</v>
       </c>
-      <c r="B454" s="55">
+      <c r="B454" s="18">
         <v>450</v>
       </c>
-      <c r="C454" s="56" t="s">
+      <c r="C454" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D454" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E454" s="55" t="s">
+      <c r="D454" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E454" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="F454" s="58">
+      <c r="F454" s="20">
         <v>44118</v>
       </c>
-      <c r="G454" s="55" t="s">
+      <c r="G454" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H454" s="59" t="s">
+      <c r="H454" s="24" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="455" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A455" s="55">
+      <c r="A455" s="18">
         <v>450</v>
       </c>
-      <c r="B455" s="55">
+      <c r="B455" s="18">
         <v>451</v>
       </c>
-      <c r="C455" s="56" t="s">
+      <c r="C455" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D455" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E455" s="55" t="s">
+      <c r="D455" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E455" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="F455" s="58">
+      <c r="F455" s="20">
         <v>44118</v>
       </c>
-      <c r="G455" s="55" t="s">
+      <c r="G455" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H455" s="59" t="s">
+      <c r="H455" s="24" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="456" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A456" s="55">
+      <c r="A456" s="18">
         <v>451</v>
       </c>
-      <c r="B456" s="55">
+      <c r="B456" s="18">
         <v>452</v>
       </c>
-      <c r="C456" s="56" t="s">
+      <c r="C456" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D456" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E456" s="55" t="s">
+      <c r="D456" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E456" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="F456" s="58">
+      <c r="F456" s="20">
         <v>44118</v>
       </c>
-      <c r="G456" s="55" t="s">
+      <c r="G456" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H456" s="59" t="s">
+      <c r="H456" s="24" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="457" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A457" s="55">
+      <c r="A457" s="18">
         <v>452</v>
       </c>
-      <c r="B457" s="55">
+      <c r="B457" s="18">
         <v>453</v>
       </c>
-      <c r="C457" s="56" t="s">
+      <c r="C457" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D457" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E457" s="55" t="s">
+      <c r="D457" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E457" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F457" s="58">
+      <c r="F457" s="20">
         <v>44118</v>
       </c>
-      <c r="G457" s="55" t="s">
+      <c r="G457" s="18" t="s">
         <v>617</v>
       </c>
-      <c r="H457" s="59" t="s">
+      <c r="H457" s="24" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="458" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A458" s="61" t="s">
+    <row r="458" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A458" s="55">
+        <v>453</v>
+      </c>
+      <c r="B458" s="55">
+        <v>454</v>
+      </c>
+      <c r="C458" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D458" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E458" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="F458" s="58">
+        <v>44119</v>
+      </c>
+      <c r="G458" s="55" t="s">
+        <v>586</v>
+      </c>
+      <c r="H458" s="59" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A459" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="B458" s="61"/>
-      <c r="C458" s="61"/>
-      <c r="D458" s="61"/>
-      <c r="E458" s="61"/>
-      <c r="F458" s="61"/>
-      <c r="G458" s="61"/>
-      <c r="H458" s="61"/>
+      <c r="B459" s="61"/>
+      <c r="C459" s="61"/>
+      <c r="D459" s="61"/>
+      <c r="E459" s="61"/>
+      <c r="F459" s="61"/>
+      <c r="G459" s="61"/>
+      <c r="H459" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A458:H458"/>
+    <mergeCell ref="A459:H459"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="D20:D21"/>

</xml_diff>

<commit_message>
patients update & ruby 2.7.2
</commit_message>
<xml_diff>
--- a/work/09_tochigi.xlsx
+++ b/work/09_tochigi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\06-01②総務G（広報チーム）\HP更新用\発生状況一覧\20201110\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Wifs507\新型コロナウイルス対策\06-01②総務G（広報チーム）\HP更新用\発生状況一覧\20201111\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,8 +15,8 @@
     <sheet name="発生状況" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">発生状況!$A$2:$I$509</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">発生状況!$A$1:$H$509</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">発生状況!$A$2:$H$511</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">発生状況!$A$1:$H$511</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">発生状況!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="669">
   <si>
     <t>栃木県内　新型コロナウイルス感染症　発生状況</t>
   </si>
@@ -5670,6 +5670,33 @@
       <t>ウツノミヤシ</t>
     </rPh>
     <rPh sb="17" eb="19">
+      <t>レイメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>50代</t>
+    <rPh sb="2" eb="3">
+      <t>ダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>高根沢町</t>
+    <rPh sb="0" eb="4">
+      <t>タカネザワマチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No.504の同僚　※宇都宮市137例目</t>
+    <rPh sb="7" eb="9">
+      <t>ドウリョウ</t>
+    </rPh>
+    <rPh sb="11" eb="15">
+      <t>ウツノミヤシ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
       <t>レイメ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -6397,11 +6424,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H509"/>
+  <dimension ref="A1:H511"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A508" sqref="A508"/>
+      <selection pane="bottomLeft" activeCell="K417" sqref="K417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -6412,8 +6439,7 @@
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
     <col min="6" max="7" width="11.625" style="3" customWidth="1"/>
     <col min="8" max="8" width="48.75" style="5" customWidth="1"/>
-    <col min="9" max="9" width="5.75" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -18733,8 +18759,8 @@
       <c r="F475" s="20">
         <v>44124</v>
       </c>
-      <c r="G475" s="18" t="s">
-        <v>583</v>
+      <c r="G475" s="20">
+        <v>44145</v>
       </c>
       <c r="H475" s="24" t="s">
         <v>639</v>
@@ -19495,125 +19521,178 @@
       </c>
     </row>
     <row r="505" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A505" s="55">
+      <c r="A505" s="18">
         <v>500</v>
       </c>
-      <c r="B505" s="55">
+      <c r="B505" s="18">
         <v>501</v>
       </c>
-      <c r="C505" s="56" t="s">
+      <c r="C505" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D505" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E505" s="55" t="s">
+      <c r="D505" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E505" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F505" s="58">
+      <c r="F505" s="20">
         <v>44144</v>
       </c>
-      <c r="G505" s="55" t="s">
+      <c r="G505" s="18" t="s">
         <v>583</v>
       </c>
-      <c r="H505" s="59" t="s">
+      <c r="H505" s="24" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="506" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A506" s="55">
+      <c r="A506" s="18">
         <v>501</v>
       </c>
-      <c r="B506" s="55">
+      <c r="B506" s="18">
         <v>502</v>
       </c>
-      <c r="C506" s="56" t="s">
+      <c r="C506" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D506" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E506" s="55" t="s">
+      <c r="D506" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E506" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F506" s="58">
+      <c r="F506" s="20">
         <v>44144</v>
       </c>
-      <c r="G506" s="55" t="s">
+      <c r="G506" s="18" t="s">
         <v>583</v>
       </c>
-      <c r="H506" s="59" t="s">
+      <c r="H506" s="24" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="507" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A507" s="55">
+      <c r="A507" s="18">
         <v>502</v>
       </c>
-      <c r="B507" s="55">
+      <c r="B507" s="18">
         <v>503</v>
       </c>
-      <c r="C507" s="56" t="s">
+      <c r="C507" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D507" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E507" s="55" t="s">
+      <c r="D507" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E507" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F507" s="58">
+      <c r="F507" s="20">
         <v>44145</v>
       </c>
-      <c r="G507" s="55" t="s">
+      <c r="G507" s="18" t="s">
         <v>583</v>
       </c>
-      <c r="H507" s="59" t="s">
+      <c r="H507" s="24" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="508" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A508" s="55">
+      <c r="A508" s="18">
         <v>503</v>
       </c>
-      <c r="B508" s="55">
+      <c r="B508" s="18">
         <v>504</v>
       </c>
-      <c r="C508" s="56" t="s">
+      <c r="C508" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D508" s="57" t="s">
+      <c r="D508" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E508" s="55" t="s">
+      <c r="E508" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F508" s="58">
+      <c r="F508" s="20">
         <v>44145</v>
       </c>
-      <c r="G508" s="55" t="s">
+      <c r="G508" s="18" t="s">
         <v>583</v>
       </c>
-      <c r="H508" s="59" t="s">
+      <c r="H508" s="24" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="509" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A509" s="61" t="s">
+    <row r="509" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A509" s="55">
+        <v>504</v>
+      </c>
+      <c r="B509" s="55">
+        <v>505</v>
+      </c>
+      <c r="C509" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D509" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E509" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="F509" s="58">
+        <v>44146</v>
+      </c>
+      <c r="G509" s="55" t="s">
+        <v>583</v>
+      </c>
+      <c r="H509" s="59" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" s="49" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A510" s="55">
+        <v>505</v>
+      </c>
+      <c r="B510" s="55">
+        <v>506</v>
+      </c>
+      <c r="C510" s="56" t="s">
+        <v>666</v>
+      </c>
+      <c r="D510" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E510" s="55" t="s">
+        <v>667</v>
+      </c>
+      <c r="F510" s="58">
+        <v>44146</v>
+      </c>
+      <c r="G510" s="55" t="s">
+        <v>583</v>
+      </c>
+      <c r="H510" s="59" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A511" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="B509" s="61"/>
-      <c r="C509" s="61"/>
-      <c r="D509" s="61"/>
-      <c r="E509" s="61"/>
-      <c r="F509" s="61"/>
-      <c r="G509" s="61"/>
-      <c r="H509" s="61"/>
+      <c r="B511" s="61"/>
+      <c r="C511" s="61"/>
+      <c r="D511" s="61"/>
+      <c r="E511" s="61"/>
+      <c r="F511" s="61"/>
+      <c r="G511" s="61"/>
+      <c r="H511" s="61"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:H511"/>
   <mergeCells count="8">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A509:H509"/>
+    <mergeCell ref="A511:H511"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="D20:D21"/>

</xml_diff>